<commit_message>
here's all the lyx files and some changes in brownian motion
</commit_message>
<xml_diff>
--- a/Financial_Modeling/training.xlsx
+++ b/Financial_Modeling/training.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhyon\PycharmProjects\financial_modeling\Git_practice\finance_project\Financial_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E010686D-8CE5-436B-BA53-3FC3B82A5740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE409FC7-D4A5-4BE7-B549-89EF7C776952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="735" windowWidth="14790" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="2" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
   <dimension ref="C2:S4002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M7" sqref="J7:M7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,6 +1083,7 @@
     <col min="9" max="9" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">

</xml_diff>